<commit_message>
updated pfm hint calibs
</commit_message>
<xml_diff>
--- a/assets/default_calibrations/pfm/20220805_pfm_55Fe109Cd137Cs_00deg_thr105_LV0d5/report_cal.xlsx
+++ b/assets/default_calibrations/pfm/20220805_pfm_55Fe109Cd137Cs_00deg_thr105_LV0d5/report_cal.xlsx
@@ -423,19 +423,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>165.3555567783817</v>
+        <v>165.3555567635691</v>
       </c>
       <c r="C2">
-        <v>0.2846692270232649</v>
+        <v>0.2846691876562966</v>
       </c>
       <c r="D2">
-        <v>16061.26764018127</v>
+        <v>16061.26764043667</v>
       </c>
       <c r="E2">
-        <v>5.279753028165413</v>
+        <v>5.279752547674532</v>
       </c>
       <c r="F2">
-        <v>25.69165583204741</v>
+        <v>25.6916558320426</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -443,19 +443,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>139.6072504166872</v>
+        <v>139.6072504570533</v>
       </c>
       <c r="C3">
-        <v>0.6975599670172852</v>
+        <v>0.6975600185550906</v>
       </c>
       <c r="D3">
-        <v>15908.76990320294</v>
+        <v>15908.76990151649</v>
       </c>
       <c r="E3">
-        <v>16.38943078414208</v>
+        <v>16.38943199105141</v>
       </c>
       <c r="F3">
-        <v>24.10412022337766</v>
+        <v>24.10412022176115</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -463,19 +463,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>163.5016479306994</v>
+        <v>163.5016479300978</v>
       </c>
       <c r="C4">
-        <v>0.5575121352096705</v>
+        <v>0.5575121346064154</v>
       </c>
       <c r="D4">
-        <v>16319.73096385813</v>
+        <v>16319.73096386248</v>
       </c>
       <c r="E4">
-        <v>13.11764207634158</v>
+        <v>13.11764206576456</v>
       </c>
       <c r="F4">
-        <v>27.03267437772932</v>
+        <v>27.03267433555539</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -483,19 +483,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>156.1865692591833</v>
+        <v>156.1865692594346</v>
       </c>
       <c r="C5">
-        <v>1.603798245537123</v>
+        <v>1.603798267071451</v>
       </c>
       <c r="D5">
-        <v>15194.13253751537</v>
+        <v>15194.13253750194</v>
       </c>
       <c r="E5">
-        <v>37.642296843719</v>
+        <v>37.64229789181613</v>
       </c>
       <c r="F5">
-        <v>93.27212608075664</v>
+        <v>93.2721262412396</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -503,19 +503,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>158.2531511392811</v>
+        <v>158.2531511392327</v>
       </c>
       <c r="C6">
-        <v>3.072507620319486</v>
+        <v>3.072507620318555</v>
       </c>
       <c r="D6">
-        <v>15768.83741563416</v>
+        <v>15768.83741563555</v>
       </c>
       <c r="E6">
-        <v>74.38800651705597</v>
+        <v>74.38800651706273</v>
       </c>
       <c r="F6">
-        <v>285.1620064079673</v>
+        <v>285.1620064079725</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -523,19 +523,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>165.8342265171293</v>
+        <v>165.8342265014746</v>
       </c>
       <c r="C7">
-        <v>0.319341079449726</v>
+        <v>0.3193411018215331</v>
       </c>
       <c r="D7">
-        <v>16005.28371012204</v>
+        <v>16005.28371039288</v>
       </c>
       <c r="E7">
-        <v>6.744170577893111</v>
+        <v>6.744170697786675</v>
       </c>
       <c r="F7">
-        <v>60.66735770353716</v>
+        <v>60.66735744914222</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -543,19 +543,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>181.0117916725171</v>
+        <v>181.0117916732895</v>
       </c>
       <c r="C8">
-        <v>0.5205962947394185</v>
+        <v>0.5205962775866592</v>
       </c>
       <c r="D8">
-        <v>15265.15431656547</v>
+        <v>15265.15431655861</v>
       </c>
       <c r="E8">
-        <v>12.3601563198359</v>
+        <v>12.36015590282881</v>
       </c>
       <c r="F8">
-        <v>36.61303459540285</v>
+        <v>36.61303471915882</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -563,19 +563,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>150.3528318242651</v>
+        <v>150.3528318236284</v>
       </c>
       <c r="C9">
-        <v>0.2849179111173014</v>
+        <v>0.2849179102249104</v>
       </c>
       <c r="D9">
-        <v>16227.57023811128</v>
+        <v>16227.57023812644</v>
       </c>
       <c r="E9">
-        <v>5.042765704393013</v>
+        <v>5.042765702586105</v>
       </c>
       <c r="F9">
-        <v>68.22698949515966</v>
+        <v>68.22698949514459</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -583,19 +583,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>173.7660132699437</v>
+        <v>173.766013283171</v>
       </c>
       <c r="C10">
-        <v>0.552181046834992</v>
+        <v>0.5521810451022284</v>
       </c>
       <c r="D10">
-        <v>15742.10729444429</v>
+        <v>15742.10729425468</v>
       </c>
       <c r="E10">
-        <v>11.95169552885455</v>
+        <v>11.95169571127901</v>
       </c>
       <c r="F10">
-        <v>49.68558692970422</v>
+        <v>49.68558771435263</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -603,19 +603,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>173.5009630243333</v>
+        <v>173.5009630243314</v>
       </c>
       <c r="C11">
-        <v>0.5478820157764552</v>
+        <v>0.547882025475509</v>
       </c>
       <c r="D11">
-        <v>15625.18933046703</v>
+        <v>15625.18933046718</v>
       </c>
       <c r="E11">
-        <v>12.51043721866772</v>
+        <v>12.51043729034678</v>
       </c>
       <c r="F11">
-        <v>34.98981970303542</v>
+        <v>34.98981970304272</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -623,19 +623,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>180.911691685131</v>
+        <v>180.9116917014853</v>
       </c>
       <c r="C12">
-        <v>0.4058337694814535</v>
+        <v>0.4058337979976063</v>
       </c>
       <c r="D12">
-        <v>16359.77000039615</v>
+        <v>16359.77000007425</v>
       </c>
       <c r="E12">
-        <v>9.082076458038047</v>
+        <v>9.082076827964704</v>
       </c>
       <c r="F12">
-        <v>31.55727805500715</v>
+        <v>31.55727865764441</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -643,19 +643,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>160.7271313665021</v>
+        <v>160.7271314308346</v>
       </c>
       <c r="C13">
-        <v>1.348511376306672</v>
+        <v>1.348511472264877</v>
       </c>
       <c r="D13">
-        <v>16273.36916664211</v>
+        <v>16273.36916510844</v>
       </c>
       <c r="E13">
-        <v>32.36940587722525</v>
+        <v>32.36940819324799</v>
       </c>
       <c r="F13">
-        <v>63.86429947015927</v>
+        <v>63.86429864249259</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -663,19 +663,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>174.1361559767714</v>
+        <v>174.1361559812643</v>
       </c>
       <c r="C14">
-        <v>0.2432124825712854</v>
+        <v>0.2432124825803772</v>
       </c>
       <c r="D14">
-        <v>15649.85958986017</v>
+        <v>15649.85958971772</v>
       </c>
       <c r="E14">
-        <v>5.810426014952576</v>
+        <v>5.810426018867526</v>
       </c>
       <c r="F14">
-        <v>13.494827717936</v>
+        <v>13.49482771395364</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -683,19 +683,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>162.9461707876154</v>
+        <v>162.9461707690149</v>
       </c>
       <c r="C15">
-        <v>0.565051462223644</v>
+        <v>0.5650514664083583</v>
       </c>
       <c r="D15">
-        <v>15895.35593747024</v>
+        <v>15895.35593825173</v>
       </c>
       <c r="E15">
-        <v>13.58091618503</v>
+        <v>13.58091634311702</v>
       </c>
       <c r="F15">
-        <v>23.06904385466094</v>
+        <v>23.06904385464799</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -703,19 +703,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>179.4649811515943</v>
+        <v>179.4649811523851</v>
       </c>
       <c r="C16">
-        <v>0.1325892966675006</v>
+        <v>0.1325893100520173</v>
       </c>
       <c r="D16">
-        <v>16119.98606179761</v>
+        <v>16119.98606177702</v>
       </c>
       <c r="E16">
-        <v>2.87362052050942</v>
+        <v>2.873620758031167</v>
       </c>
       <c r="F16">
-        <v>3.093313421336881</v>
+        <v>3.093313408683669</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -723,19 +723,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>161.6011287436866</v>
+        <v>161.6011287244663</v>
       </c>
       <c r="C17">
-        <v>0.3736736369963338</v>
+        <v>0.373673676413299</v>
       </c>
       <c r="D17">
-        <v>15604.20579202414</v>
+        <v>15604.2057924492</v>
       </c>
       <c r="E17">
-        <v>8.925012874180103</v>
+        <v>8.925013716720652</v>
       </c>
       <c r="F17">
-        <v>16.91599702674808</v>
+        <v>16.91599678853551</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -743,19 +743,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>157.8215209473435</v>
+        <v>157.8215210510754</v>
       </c>
       <c r="C18">
-        <v>0.738430448085843</v>
+        <v>0.7384304805637124</v>
       </c>
       <c r="D18">
-        <v>15462.144604282</v>
+        <v>15462.14460155584</v>
       </c>
       <c r="E18">
-        <v>16.95282229094407</v>
+        <v>16.95282226228182</v>
       </c>
       <c r="F18">
-        <v>48.91461894171707</v>
+        <v>48.91461879028991</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -763,19 +763,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>173.8890136755244</v>
+        <v>173.8890136465911</v>
       </c>
       <c r="C19">
-        <v>0.6840706744214821</v>
+        <v>0.6840706560502832</v>
       </c>
       <c r="D19">
-        <v>15786.58234887494</v>
+        <v>15786.58234958163</v>
       </c>
       <c r="E19">
-        <v>16.26920613692052</v>
+        <v>16.26920586784371</v>
       </c>
       <c r="F19">
-        <v>106.7918240380883</v>
+        <v>106.7918240676572</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -783,19 +783,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>156.4296063719575</v>
+        <v>156.4296063713263</v>
       </c>
       <c r="C20">
-        <v>1.011645106128324</v>
+        <v>1.0116451953238</v>
       </c>
       <c r="D20">
-        <v>15374.82496551728</v>
+        <v>15374.82496553574</v>
       </c>
       <c r="E20">
-        <v>24.8153176532151</v>
+        <v>24.8153183299689</v>
       </c>
       <c r="F20">
-        <v>50.18582508911116</v>
+        <v>50.18582481467617</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -803,19 +803,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>162.1411892141386</v>
+        <v>162.1411892014549</v>
       </c>
       <c r="C21">
-        <v>0.9540397919499957</v>
+        <v>0.9540397898880713</v>
       </c>
       <c r="D21">
-        <v>16344.1097677265</v>
+        <v>16344.10976802389</v>
       </c>
       <c r="E21">
-        <v>22.67596647864256</v>
+        <v>22.67596643605739</v>
       </c>
       <c r="F21">
-        <v>131.1484682100266</v>
+        <v>131.1484677119572</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -823,19 +823,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>177.4177150438345</v>
+        <v>177.4177150411288</v>
       </c>
       <c r="C22">
-        <v>0.3062765214056597</v>
+        <v>0.3062765224084864</v>
       </c>
       <c r="D22">
-        <v>16445.92243292895</v>
+        <v>16445.92243299438</v>
       </c>
       <c r="E22">
-        <v>6.632530680602844</v>
+        <v>6.632530704185688</v>
       </c>
       <c r="F22">
-        <v>36.31623618129046</v>
+        <v>36.3162361544424</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -843,19 +843,19 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>181.4088251490442</v>
+        <v>181.4088251483717</v>
       </c>
       <c r="C23">
-        <v>0.09254025773488246</v>
+        <v>0.09254025788483736</v>
       </c>
       <c r="D23">
-        <v>15884.29157091492</v>
+        <v>15884.29157092712</v>
       </c>
       <c r="E23">
-        <v>1.802224246576747</v>
+        <v>1.802224243653649</v>
       </c>
       <c r="F23">
-        <v>4.405009035837734</v>
+        <v>4.405009081073465</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -863,19 +863,19 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>173.9579093276291</v>
+        <v>173.9579093163665</v>
       </c>
       <c r="C24">
-        <v>0.2021083737289559</v>
+        <v>0.2021083732270272</v>
       </c>
       <c r="D24">
-        <v>15605.19691228743</v>
+        <v>15605.19691255554</v>
       </c>
       <c r="E24">
-        <v>4.075390872080328</v>
+        <v>4.075390866059569</v>
       </c>
       <c r="F24">
-        <v>20.9489832025012</v>
+        <v>20.94898314412572</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -886,16 +886,16 @@
         <v>172.8134323642025</v>
       </c>
       <c r="C25">
-        <v>0.3513843850725303</v>
+        <v>0.3513843820946633</v>
       </c>
       <c r="D25">
         <v>16438.32955428729</v>
       </c>
       <c r="E25">
-        <v>7.407013932406222</v>
+        <v>7.407013946819538</v>
       </c>
       <c r="F25">
-        <v>51.77470721143483</v>
+        <v>51.77470721138916</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -903,19 +903,19 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>170.4149904241394</v>
+        <v>170.4149904275646</v>
       </c>
       <c r="C26">
-        <v>0.2457854383427028</v>
+        <v>0.2457854575883802</v>
       </c>
       <c r="D26">
-        <v>16273.55617612543</v>
+        <v>16273.55617604288</v>
       </c>
       <c r="E26">
-        <v>5.80633376866415</v>
+        <v>5.806333909483022</v>
       </c>
       <c r="F26">
-        <v>14.0570914041154</v>
+        <v>14.05709140600103</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -923,19 +923,19 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>164.0448751575469</v>
+        <v>164.0448751557498</v>
       </c>
       <c r="C27">
-        <v>1.09013587130354</v>
+        <v>1.090135807710684</v>
       </c>
       <c r="D27">
-        <v>15914.74772498174</v>
+        <v>15914.74772499928</v>
       </c>
       <c r="E27">
-        <v>26.70621492885168</v>
+        <v>26.70621337304537</v>
       </c>
       <c r="F27">
-        <v>112.1387121094687</v>
+        <v>112.1387117400039</v>
       </c>
     </row>
   </sheetData>
@@ -976,19 +976,19 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>148.5025879081056</v>
+        <v>148.502587909038</v>
       </c>
       <c r="C2">
-        <v>1.578839161494464</v>
+        <v>1.578839159488463</v>
       </c>
       <c r="D2">
-        <v>15941.21948853314</v>
+        <v>15941.21948854258</v>
       </c>
       <c r="E2">
-        <v>34.13097852562201</v>
+        <v>34.13097847990397</v>
       </c>
       <c r="F2">
-        <v>236.5942132682759</v>
+        <v>236.5942126223916</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -996,19 +996,19 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>173.8108250267786</v>
+        <v>173.8108250247425</v>
       </c>
       <c r="C3">
-        <v>0.3287151442940588</v>
+        <v>0.3287151371143996</v>
       </c>
       <c r="D3">
-        <v>15875.07682764683</v>
+        <v>15875.07682769893</v>
       </c>
       <c r="E3">
-        <v>7.672686152486775</v>
+        <v>7.672685973999883</v>
       </c>
       <c r="F3">
-        <v>8.021455922582506</v>
+        <v>8.02145586620472</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1016,19 +1016,19 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>195.8629325358436</v>
+        <v>195.8629325294889</v>
       </c>
       <c r="C4">
-        <v>0.2513030854943982</v>
+        <v>0.2513030904617201</v>
       </c>
       <c r="D4">
-        <v>15649.31775441281</v>
+        <v>15649.31775458422</v>
       </c>
       <c r="E4">
-        <v>5.574594107437024</v>
+        <v>5.574594074670763</v>
       </c>
       <c r="F4">
-        <v>13.98858735973592</v>
+        <v>13.98858723650079</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1036,19 +1036,19 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>174.8276505502515</v>
+        <v>174.8276505264849</v>
       </c>
       <c r="C5">
-        <v>0.5998969976570745</v>
+        <v>0.5998969954818963</v>
       </c>
       <c r="D5">
-        <v>15307.52552839412</v>
+        <v>15307.52552882791</v>
       </c>
       <c r="E5">
-        <v>11.03426262391646</v>
+        <v>11.03426262153544</v>
       </c>
       <c r="F5">
-        <v>61.20666716010857</v>
+        <v>61.20666721137935</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1056,19 +1056,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>165.3891700157326</v>
+        <v>165.3891700370743</v>
       </c>
       <c r="C6">
-        <v>0.9956093882920506</v>
+        <v>0.9956093155149044</v>
       </c>
       <c r="D6">
-        <v>15544.93852412435</v>
+        <v>15544.93852377566</v>
       </c>
       <c r="E6">
-        <v>22.95836882842445</v>
+        <v>22.95836723860815</v>
       </c>
       <c r="F6">
-        <v>180.8905604380899</v>
+        <v>180.8905622824549</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1076,19 +1076,19 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>154.8293570292866</v>
+        <v>154.8293570806376</v>
       </c>
       <c r="C7">
-        <v>0.77202469023874</v>
+        <v>0.772024631696736</v>
       </c>
       <c r="D7">
-        <v>15296.04344498345</v>
+        <v>15296.04344365831</v>
       </c>
       <c r="E7">
-        <v>16.89002470147189</v>
+        <v>16.89002427586968</v>
       </c>
       <c r="F7">
-        <v>49.59683849403886</v>
+        <v>49.59683849404696</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1096,19 +1096,19 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>152.5436394657781</v>
+        <v>152.5436394657759</v>
       </c>
       <c r="C8">
-        <v>0.6683381081394096</v>
+        <v>0.6683380979816256</v>
       </c>
       <c r="D8">
-        <v>15406.47540340351</v>
+        <v>15406.47540340357</v>
       </c>
       <c r="E8">
-        <v>14.04930077281122</v>
+        <v>14.04930070064566</v>
       </c>
       <c r="F8">
-        <v>128.0253399187214</v>
+        <v>128.0253399186954</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1116,19 +1116,19 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>193.7268941275546</v>
+        <v>193.7268941289194</v>
       </c>
       <c r="C9">
-        <v>0.06243159491193431</v>
+        <v>0.06243159088983271</v>
       </c>
       <c r="D9">
-        <v>16535.01355541142</v>
+        <v>16535.01355536563</v>
       </c>
       <c r="E9">
-        <v>1.34064833820851</v>
+        <v>1.340648242248411</v>
       </c>
       <c r="F9">
-        <v>1.459463832506435</v>
+        <v>1.459463832506168</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1136,19 +1136,19 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>148.5786465669864</v>
+        <v>148.5786465032412</v>
       </c>
       <c r="C10">
-        <v>0.6946221354502484</v>
+        <v>0.6946221417615572</v>
       </c>
       <c r="D10">
-        <v>15767.95676000843</v>
+        <v>15767.95676121488</v>
       </c>
       <c r="E10">
-        <v>14.53105243601993</v>
+        <v>14.53105240526651</v>
       </c>
       <c r="F10">
-        <v>99.19219239600949</v>
+        <v>99.19219225830258</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1156,19 +1156,19 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>175.6144766369117</v>
+        <v>175.6144766409544</v>
       </c>
       <c r="C11">
-        <v>0.2997850967013784</v>
+        <v>0.2997851196164268</v>
       </c>
       <c r="D11">
-        <v>15801.71960456072</v>
+        <v>15801.71960448135</v>
       </c>
       <c r="E11">
-        <v>6.168636861816789</v>
+        <v>6.168637371597363</v>
       </c>
       <c r="F11">
-        <v>27.75672367575289</v>
+        <v>27.75672381284098</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1176,19 +1176,19 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>175.6589487779829</v>
+        <v>175.6589487492781</v>
       </c>
       <c r="C12">
-        <v>0.9074411218827153</v>
+        <v>0.9074411777256984</v>
       </c>
       <c r="D12">
-        <v>15979.88840543996</v>
+        <v>15979.88840617207</v>
       </c>
       <c r="E12">
-        <v>20.8725756924819</v>
+        <v>20.87257640658703</v>
       </c>
       <c r="F12">
-        <v>128.7680026213337</v>
+        <v>128.7680026333378</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1196,19 +1196,19 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>179.8028466348699</v>
+        <v>179.8028466523587</v>
       </c>
       <c r="C13">
-        <v>0.2640337341448281</v>
+        <v>0.2640337341701108</v>
       </c>
       <c r="D13">
-        <v>15295.14445074299</v>
+        <v>15295.14445043503</v>
       </c>
       <c r="E13">
-        <v>5.396116861127545</v>
+        <v>5.396116861020482</v>
       </c>
       <c r="F13">
-        <v>14.36452208926037</v>
+        <v>14.36452208926575</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1216,19 +1216,19 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>156.891763921957</v>
+        <v>156.8917638362342</v>
       </c>
       <c r="C14">
-        <v>0.7661495493865463</v>
+        <v>0.7661495375875202</v>
       </c>
       <c r="D14">
-        <v>15847.46887172379</v>
+        <v>15847.46887345899</v>
       </c>
       <c r="E14">
-        <v>16.52474611381018</v>
+        <v>16.52474602515995</v>
       </c>
       <c r="F14">
-        <v>75.956681764789</v>
+        <v>75.95668177731095</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1236,19 +1236,19 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>166.7168635824987</v>
+        <v>166.7168635685393</v>
       </c>
       <c r="C15">
-        <v>0.9021488153715784</v>
+        <v>0.9021488188303001</v>
       </c>
       <c r="D15">
-        <v>15449.5968851689</v>
+        <v>15449.59688546296</v>
       </c>
       <c r="E15">
-        <v>21.32051695003903</v>
+        <v>21.32051709283647</v>
       </c>
       <c r="F15">
-        <v>48.81892633496172</v>
+        <v>48.81892651328978</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1256,19 +1256,19 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>168.1224897844696</v>
+        <v>168.1224898123581</v>
       </c>
       <c r="C16">
-        <v>0.5813400067309614</v>
+        <v>0.5813399740075451</v>
       </c>
       <c r="D16">
-        <v>15865.67704039033</v>
+        <v>15865.67703973779</v>
       </c>
       <c r="E16">
-        <v>13.44451427907379</v>
+        <v>13.4445141413426</v>
       </c>
       <c r="F16">
-        <v>38.99147024596071</v>
+        <v>38.99147037597575</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1276,19 +1276,19 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>170.8032479501825</v>
+        <v>170.8032479635995</v>
       </c>
       <c r="C17">
-        <v>0.3308682556547427</v>
+        <v>0.3308682547713362</v>
       </c>
       <c r="D17">
-        <v>16259.07979141054</v>
+        <v>16259.07979130049</v>
       </c>
       <c r="E17">
-        <v>7.355219692160523</v>
+        <v>7.355219679773115</v>
       </c>
       <c r="F17">
-        <v>14.54778835465532</v>
+        <v>14.54778835298432</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1296,19 +1296,19 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>142.2160089383816</v>
+        <v>142.2160089372136</v>
       </c>
       <c r="C18">
-        <v>0.4989035077091989</v>
+        <v>0.4989035012339962</v>
       </c>
       <c r="D18">
-        <v>16147.88112923746</v>
+        <v>16147.88112927264</v>
       </c>
       <c r="E18">
-        <v>9.754553328670623</v>
+        <v>9.754553308590298</v>
       </c>
       <c r="F18">
-        <v>134.8843301946939</v>
+        <v>134.884329592876</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1316,19 +1316,19 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>165.486508425444</v>
+        <v>165.4865084110864</v>
       </c>
       <c r="C19">
-        <v>0.8153933492545575</v>
+        <v>0.8153933505472399</v>
       </c>
       <c r="D19">
-        <v>15561.87106700125</v>
+        <v>15561.87106803097</v>
       </c>
       <c r="E19">
-        <v>20.10043066798013</v>
+        <v>20.10043070291245</v>
       </c>
       <c r="F19">
-        <v>53.50903973286425</v>
+        <v>53.50903991589366</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1336,19 +1336,19 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>164.2730737362967</v>
+        <v>164.273073717635</v>
       </c>
       <c r="C20">
-        <v>0.4123000083678477</v>
+        <v>0.4123000463208827</v>
       </c>
       <c r="D20">
-        <v>16559.41228910924</v>
+        <v>16559.41228957148</v>
       </c>
       <c r="E20">
-        <v>9.580818630319975</v>
+        <v>9.580819018787256</v>
       </c>
       <c r="F20">
-        <v>22.90739334956659</v>
+        <v>22.90739336773224</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1356,19 +1356,19 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>150.6927927288538</v>
+        <v>150.692792727735</v>
       </c>
       <c r="C21">
-        <v>0.8672397385774478</v>
+        <v>0.8672396221956541</v>
       </c>
       <c r="D21">
-        <v>16009.94176374759</v>
+        <v>16009.94176375631</v>
       </c>
       <c r="E21">
-        <v>20.53856514167941</v>
+        <v>20.53856337013933</v>
       </c>
       <c r="F21">
-        <v>140.3566890710709</v>
+        <v>140.3566889244642</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1376,19 +1376,19 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>179.0708248728043</v>
+        <v>179.0708248810057</v>
       </c>
       <c r="C22">
-        <v>0.193179754075546</v>
+        <v>0.1931797572522758</v>
       </c>
       <c r="D22">
-        <v>16366.32996039231</v>
+        <v>16366.3299601295</v>
       </c>
       <c r="E22">
-        <v>3.997783941435159</v>
+        <v>3.997783946467878</v>
       </c>
       <c r="F22">
-        <v>5.699929382709549</v>
+        <v>5.69992938252555</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1396,19 +1396,19 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>164.9481264626403</v>
+        <v>164.9481265018553</v>
       </c>
       <c r="C23">
-        <v>0.4433481014384963</v>
+        <v>0.4433481036834265</v>
       </c>
       <c r="D23">
-        <v>16079.80504761562</v>
+        <v>16079.80504666117</v>
       </c>
       <c r="E23">
-        <v>9.776718979124782</v>
+        <v>9.776719417014887</v>
       </c>
       <c r="F23">
-        <v>26.82518288812523</v>
+        <v>26.82518288813202</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1416,19 +1416,19 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>177.8502732576532</v>
+        <v>177.8502732552364</v>
       </c>
       <c r="C24">
-        <v>0.4535241885547739</v>
+        <v>0.4535241676569395</v>
       </c>
       <c r="D24">
-        <v>15864.00455351668</v>
+        <v>15864.00455353332</v>
       </c>
       <c r="E24">
-        <v>10.96917770821015</v>
+        <v>10.96917763287144</v>
       </c>
       <c r="F24">
-        <v>26.13485775878067</v>
+        <v>26.13485739964504</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1436,19 +1436,19 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>153.4662843544441</v>
+        <v>153.4662842968795</v>
       </c>
       <c r="C25">
-        <v>1.258153707102274</v>
+        <v>1.258153658488007</v>
       </c>
       <c r="D25">
-        <v>15044.73990052375</v>
+        <v>15044.73990188623</v>
       </c>
       <c r="E25">
-        <v>27.66646866779571</v>
+        <v>27.66646771804171</v>
       </c>
       <c r="F25">
-        <v>147.7247345576196</v>
+        <v>147.7247345078987</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1456,19 +1456,19 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>177.8925715918958</v>
+        <v>177.8925715915958</v>
       </c>
       <c r="C26">
-        <v>0.9944296454369675</v>
+        <v>0.9944296452076625</v>
       </c>
       <c r="D26">
-        <v>15261.20730105257</v>
+        <v>15261.20730105987</v>
       </c>
       <c r="E26">
-        <v>22.77873403652234</v>
+        <v>22.77873403070334</v>
       </c>
       <c r="F26">
-        <v>89.51226409856261</v>
+        <v>89.512264107273</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1476,19 +1476,19 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>171.8461103907629</v>
+        <v>171.8461104205145</v>
       </c>
       <c r="C27">
-        <v>0.6623285259832966</v>
+        <v>0.662328528631962</v>
       </c>
       <c r="D27">
-        <v>15619.46040709125</v>
+        <v>15619.46040647828</v>
       </c>
       <c r="E27">
-        <v>15.3593015831454</v>
+        <v>15.3593016493317</v>
       </c>
       <c r="F27">
-        <v>86.07680636437571</v>
+        <v>86.07680637099553</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1496,19 +1496,19 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>168.0150408573572</v>
+        <v>168.0150408575198</v>
       </c>
       <c r="C28">
-        <v>0.5933419360696421</v>
+        <v>0.5933419408551918</v>
       </c>
       <c r="D28">
-        <v>16358.98775720548</v>
+        <v>16358.98775743032</v>
       </c>
       <c r="E28">
-        <v>12.19121255039765</v>
+        <v>12.19121256471178</v>
       </c>
       <c r="F28">
-        <v>31.89367462754345</v>
+        <v>31.8936746277585</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1516,19 +1516,19 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>179.5542413498092</v>
+        <v>179.5542413527125</v>
       </c>
       <c r="C29">
-        <v>0.3402092176182485</v>
+        <v>0.3402092213703666</v>
       </c>
       <c r="D29">
-        <v>16311.58472712514</v>
+        <v>16311.58472708143</v>
       </c>
       <c r="E29">
-        <v>7.633409571689358</v>
+        <v>7.633409965349602</v>
       </c>
       <c r="F29">
-        <v>30.70003913274148</v>
+        <v>30.70003866363326</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1536,19 +1536,19 @@
         <v>31</v>
       </c>
       <c r="B30">
-        <v>159.2430262526028</v>
+        <v>159.2430262358137</v>
       </c>
       <c r="C30">
-        <v>0.4607314680202018</v>
+        <v>0.4607314768616557</v>
       </c>
       <c r="D30">
-        <v>15693.84491146197</v>
+        <v>15693.84491162991</v>
       </c>
       <c r="E30">
-        <v>8.414603227006117</v>
+        <v>8.414603860232351</v>
       </c>
       <c r="F30">
-        <v>47.93188525285125</v>
+        <v>47.93188525286256</v>
       </c>
     </row>
   </sheetData>
@@ -1589,19 +1589,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>167.7706790839382</v>
+        <v>167.770679057192</v>
       </c>
       <c r="C2">
-        <v>0.7426877154642021</v>
+        <v>0.7426877615758598</v>
       </c>
       <c r="D2">
-        <v>15764.2806003616</v>
+        <v>15764.28060096812</v>
       </c>
       <c r="E2">
-        <v>16.49596568144135</v>
+        <v>16.49596688100667</v>
       </c>
       <c r="F2">
-        <v>19.61520088712115</v>
+        <v>19.61520086407364</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1609,19 +1609,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>180.1813675929337</v>
+        <v>180.1813675711007</v>
       </c>
       <c r="C3">
-        <v>0.2912982935751612</v>
+        <v>0.2912982756761118</v>
       </c>
       <c r="D3">
-        <v>16386.36328463112</v>
+        <v>16386.36328504416</v>
       </c>
       <c r="E3">
-        <v>6.139293158326009</v>
+        <v>6.139293016310234</v>
       </c>
       <c r="F3">
-        <v>8.279178597420842</v>
+        <v>8.279178557516769</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1629,19 +1629,19 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>182.1474269947834</v>
+        <v>182.1474269822216</v>
       </c>
       <c r="C4">
-        <v>0.2807964552900579</v>
+        <v>0.2807964507845391</v>
       </c>
       <c r="D4">
-        <v>15941.89386864947</v>
+        <v>15941.89386885164</v>
       </c>
       <c r="E4">
-        <v>5.409405106146454</v>
+        <v>5.409405049894746</v>
       </c>
       <c r="F4">
-        <v>24.8244927576987</v>
+        <v>24.82449276803917</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1649,19 +1649,19 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>185.5325210809104</v>
+        <v>185.5325210812663</v>
       </c>
       <c r="C5">
-        <v>0.1487488574041065</v>
+        <v>0.1487488513855547</v>
       </c>
       <c r="D5">
-        <v>15633.0365589255</v>
+        <v>15633.03655892528</v>
       </c>
       <c r="E5">
-        <v>3.025589713353915</v>
+        <v>3.025589714419464</v>
       </c>
       <c r="F5">
-        <v>4.621089032647842</v>
+        <v>4.62108897447085</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1669,19 +1669,19 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>162.7996841734431</v>
+        <v>162.7996841749309</v>
       </c>
       <c r="C6">
-        <v>0.3118010185359575</v>
+        <v>0.3118009938208117</v>
       </c>
       <c r="D6">
-        <v>15723.94336505372</v>
+        <v>15723.9433650115</v>
       </c>
       <c r="E6">
-        <v>6.464122188202781</v>
+        <v>6.464121633761429</v>
       </c>
       <c r="F6">
-        <v>44.53379848867451</v>
+        <v>44.53379848856225</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1689,19 +1689,19 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>163.5660825453511</v>
+        <v>163.5660826076358</v>
       </c>
       <c r="C7">
-        <v>0.8122835662553372</v>
+        <v>0.8122835987843837</v>
       </c>
       <c r="D7">
-        <v>15791.68890023894</v>
+        <v>15791.68889907413</v>
       </c>
       <c r="E7">
-        <v>17.26865127875488</v>
+        <v>17.26865232818811</v>
       </c>
       <c r="F7">
-        <v>86.25885177452132</v>
+        <v>86.25885179881061</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1709,19 +1709,19 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>193.8202231281238</v>
+        <v>193.8202231419827</v>
       </c>
       <c r="C8">
-        <v>0.1350944208714706</v>
+        <v>0.135094420881081</v>
       </c>
       <c r="D8">
-        <v>15787.78662472148</v>
+        <v>15787.78662437969</v>
       </c>
       <c r="E8">
-        <v>2.862820694915001</v>
+        <v>2.862820694852527</v>
       </c>
       <c r="F8">
-        <v>6.91867070619751</v>
+        <v>6.918670706195258</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1729,19 +1729,19 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>157.8074139433019</v>
+        <v>157.8074139415925</v>
       </c>
       <c r="C9">
-        <v>0.6084200812807201</v>
+        <v>0.6084200976072157</v>
       </c>
       <c r="D9">
-        <v>16026.85608922727</v>
+        <v>16026.85608923349</v>
       </c>
       <c r="E9">
-        <v>12.90155329773936</v>
+        <v>12.90155350965264</v>
       </c>
       <c r="F9">
-        <v>195.6698318839341</v>
+        <v>195.6698356001656</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1749,19 +1749,19 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>145.9097855979078</v>
+        <v>145.9097854987005</v>
       </c>
       <c r="C10">
-        <v>1.102742843177576</v>
+        <v>1.10274275486316</v>
       </c>
       <c r="D10">
-        <v>15218.98442287378</v>
+        <v>15218.98442476637</v>
       </c>
       <c r="E10">
-        <v>23.93427920801889</v>
+        <v>23.93427856544583</v>
       </c>
       <c r="F10">
-        <v>258.4143803290579</v>
+        <v>258.4143799005406</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1769,19 +1769,19 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>181.771112720668</v>
+        <v>181.7711127379665</v>
       </c>
       <c r="C11">
-        <v>0.2792581245126849</v>
+        <v>0.2792581105227537</v>
       </c>
       <c r="D11">
-        <v>16032.56411553865</v>
+        <v>16032.56411511088</v>
       </c>
       <c r="E11">
-        <v>6.789864753887293</v>
+        <v>6.789864415693558</v>
       </c>
       <c r="F11">
-        <v>6.105377855557889</v>
+        <v>6.105377855561986</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1789,19 +1789,19 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>170.8431416745538</v>
+        <v>170.8431416789138</v>
       </c>
       <c r="C12">
-        <v>0.3454006479649936</v>
+        <v>0.3454006191676415</v>
       </c>
       <c r="D12">
-        <v>15911.3842206271</v>
+        <v>15911.38422045919</v>
       </c>
       <c r="E12">
-        <v>7.836380711027702</v>
+        <v>7.836380023338776</v>
       </c>
       <c r="F12">
-        <v>24.7878905923126</v>
+        <v>24.78789059054075</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1812,13 +1812,13 @@
         <v>192.1903690925105</v>
       </c>
       <c r="C13">
-        <v>0.07511576333940567</v>
+        <v>0.07511576333944392</v>
       </c>
       <c r="D13">
         <v>15931.04228060262</v>
       </c>
       <c r="E13">
-        <v>1.511410122379984</v>
+        <v>1.511410122379947</v>
       </c>
       <c r="F13">
         <v>1.828248269164315</v>
@@ -1829,19 +1829,19 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>165.422232649417</v>
+        <v>165.4222326447892</v>
       </c>
       <c r="C14">
-        <v>0.5620085649739656</v>
+        <v>0.5620085334856478</v>
       </c>
       <c r="D14">
-        <v>15186.7392612646</v>
+        <v>15186.73926135945</v>
       </c>
       <c r="E14">
-        <v>9.817438964872849</v>
+        <v>9.8174384761217</v>
       </c>
       <c r="F14">
-        <v>128.6087197751836</v>
+        <v>128.6087197751612</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1849,19 +1849,19 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>175.607239881573</v>
+        <v>175.6072398415862</v>
       </c>
       <c r="C15">
-        <v>0.789955781970342</v>
+        <v>0.7899559177865025</v>
       </c>
       <c r="D15">
-        <v>15759.82659591317</v>
+        <v>15759.82659688391</v>
       </c>
       <c r="E15">
-        <v>18.74830201260323</v>
+        <v>18.74830452560883</v>
       </c>
       <c r="F15">
-        <v>12.9731723603238</v>
+        <v>12.97317238907071</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1869,19 +1869,19 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>152.7403617757381</v>
+        <v>152.7403617770977</v>
       </c>
       <c r="C16">
-        <v>0.7330509884622322</v>
+        <v>0.7330510390038325</v>
       </c>
       <c r="D16">
-        <v>15436.34902745768</v>
+        <v>15436.34902742429</v>
       </c>
       <c r="E16">
-        <v>14.50067320854745</v>
+        <v>14.5006736635176</v>
       </c>
       <c r="F16">
-        <v>80.54482855627167</v>
+        <v>80.54482854051138</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1889,19 +1889,19 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>165.8224503603846</v>
+        <v>165.8224503603895</v>
       </c>
       <c r="C17">
-        <v>0.3995737624717414</v>
+        <v>0.3995737933553934</v>
       </c>
       <c r="D17">
-        <v>15616.24554806656</v>
+        <v>15616.24554806645</v>
       </c>
       <c r="E17">
-        <v>9.315126814506936</v>
+        <v>9.31512755357031</v>
       </c>
       <c r="F17">
-        <v>32.31559254657797</v>
+        <v>32.31559254658934</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1909,19 +1909,19 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>175.2313358913865</v>
+        <v>175.231335836978</v>
       </c>
       <c r="C18">
-        <v>0.6782443044933205</v>
+        <v>0.6782443017133444</v>
       </c>
       <c r="D18">
-        <v>15173.0961975248</v>
+        <v>15173.0961992629</v>
       </c>
       <c r="E18">
-        <v>16.65757883848176</v>
+        <v>16.65757877594996</v>
       </c>
       <c r="F18">
-        <v>15.81008054823251</v>
+        <v>15.8100805533379</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1929,19 +1929,19 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>169.6756286832971</v>
+        <v>169.6756286858325</v>
       </c>
       <c r="C19">
-        <v>0.4167778640880167</v>
+        <v>0.4167778653207403</v>
       </c>
       <c r="D19">
-        <v>15063.94196791119</v>
+        <v>15063.94196785586</v>
       </c>
       <c r="E19">
-        <v>8.098848623212602</v>
+        <v>8.098848623345578</v>
       </c>
       <c r="F19">
-        <v>97.19154251699057</v>
+        <v>97.19154251700469</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1949,19 +1949,19 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>156.8009749918776</v>
+        <v>156.8009749557242</v>
       </c>
       <c r="C20">
-        <v>0.4224762824289987</v>
+        <v>0.4224763138137543</v>
       </c>
       <c r="D20">
-        <v>15596.45845795572</v>
+        <v>15596.4584584101</v>
       </c>
       <c r="E20">
-        <v>9.476772754185571</v>
+        <v>9.476772930506543</v>
       </c>
       <c r="F20">
-        <v>63.19316831326363</v>
+        <v>63.19316767478804</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1969,19 +1969,19 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>162.5962629375683</v>
+        <v>162.5962629385934</v>
       </c>
       <c r="C21">
-        <v>0.3910539201480269</v>
+        <v>0.3910539192775291</v>
       </c>
       <c r="D21">
-        <v>15355.82358756456</v>
+        <v>15355.8235875395</v>
       </c>
       <c r="E21">
-        <v>7.176782506118596</v>
+        <v>7.1767824900217</v>
       </c>
       <c r="F21">
-        <v>67.1627669548847</v>
+        <v>67.16276692882546</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1989,19 +1989,19 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>185.948917214941</v>
+        <v>185.9489172324029</v>
       </c>
       <c r="C22">
-        <v>0.3223169359265571</v>
+        <v>0.3223169600054015</v>
       </c>
       <c r="D22">
-        <v>15837.19826221625</v>
+        <v>15837.19826164148</v>
       </c>
       <c r="E22">
-        <v>7.714764065505149</v>
+        <v>7.714764265713296</v>
       </c>
       <c r="F22">
-        <v>14.73473459085561</v>
+        <v>14.73473459084995</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2009,19 +2009,19 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>177.1212819992922</v>
+        <v>177.1212819976589</v>
       </c>
       <c r="C23">
-        <v>1.487803476384635</v>
+        <v>1.487803496985417</v>
       </c>
       <c r="D23">
-        <v>16276.41351037473</v>
+        <v>16276.41351041403</v>
       </c>
       <c r="E23">
-        <v>35.4586178031685</v>
+        <v>35.45861830185316</v>
       </c>
       <c r="F23">
-        <v>36.74010282919431</v>
+        <v>36.74010285332259</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2029,19 +2029,19 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>177.3044335957176</v>
+        <v>177.3044336062154</v>
       </c>
       <c r="C24">
-        <v>0.5898796887579612</v>
+        <v>0.5898796461465388</v>
       </c>
       <c r="D24">
-        <v>15631.2208729104</v>
+        <v>15631.2208727448</v>
       </c>
       <c r="E24">
-        <v>13.45318489201052</v>
+        <v>13.45318445039226</v>
       </c>
       <c r="F24">
-        <v>87.38947127702184</v>
+        <v>87.38947130353509</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2049,19 +2049,19 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>173.0584844454593</v>
+        <v>173.0584844222172</v>
       </c>
       <c r="C25">
-        <v>0.3425340596009137</v>
+        <v>0.3425340616604497</v>
       </c>
       <c r="D25">
-        <v>16635.93155695416</v>
+        <v>16635.93155735099</v>
       </c>
       <c r="E25">
-        <v>6.829320512534189</v>
+        <v>6.829320573969085</v>
       </c>
       <c r="F25">
-        <v>18.51035382174368</v>
+        <v>18.51035382598999</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2069,19 +2069,19 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>152.7985164378831</v>
+        <v>152.7985163985266</v>
       </c>
       <c r="C26">
-        <v>0.8285460750501235</v>
+        <v>0.8285460040806215</v>
       </c>
       <c r="D26">
-        <v>16060.81297636092</v>
+        <v>16060.81297676733</v>
       </c>
       <c r="E26">
-        <v>19.51462364408277</v>
+        <v>19.51462308624841</v>
       </c>
       <c r="F26">
-        <v>58.44398773833747</v>
+        <v>58.44398809048896</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2089,19 +2089,19 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>159.6822401036712</v>
+        <v>159.6822400729786</v>
       </c>
       <c r="C27">
-        <v>0.4668391116243782</v>
+        <v>0.466839150512486</v>
       </c>
       <c r="D27">
-        <v>15954.00947481313</v>
+        <v>15954.00947502699</v>
       </c>
       <c r="E27">
-        <v>10.88296769515963</v>
+        <v>10.882967998498</v>
       </c>
       <c r="F27">
-        <v>26.70540720330167</v>
+        <v>26.70540717688977</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2109,19 +2109,19 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>165.6005971971486</v>
+        <v>165.6005972342423</v>
       </c>
       <c r="C28">
-        <v>0.6560992504622416</v>
+        <v>0.6560993113923425</v>
       </c>
       <c r="D28">
-        <v>15560.48848797856</v>
+        <v>15560.48848712124</v>
       </c>
       <c r="E28">
-        <v>13.54771402880963</v>
+        <v>13.54771525408131</v>
       </c>
       <c r="F28">
-        <v>38.17258091842361</v>
+        <v>38.17258091843328</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2129,19 +2129,19 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>156.9725909299119</v>
+        <v>156.9725909220148</v>
       </c>
       <c r="C29">
-        <v>0.7105000054197251</v>
+        <v>0.7105000454827682</v>
       </c>
       <c r="D29">
-        <v>15377.46620128511</v>
+        <v>15377.46620168833</v>
       </c>
       <c r="E29">
-        <v>15.06834485934022</v>
+        <v>15.06834560438418</v>
       </c>
       <c r="F29">
-        <v>84.07272463951817</v>
+        <v>84.07272463953169</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2149,19 +2149,19 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>160.8865212148591</v>
+        <v>160.8865211810456</v>
       </c>
       <c r="C30">
-        <v>0.5687655721552231</v>
+        <v>0.5687656122554386</v>
       </c>
       <c r="D30">
-        <v>16180.56228226239</v>
+        <v>16180.56228326185</v>
       </c>
       <c r="E30">
-        <v>12.60081261493291</v>
+        <v>12.60081282679256</v>
       </c>
       <c r="F30">
-        <v>67.40443353992069</v>
+        <v>67.40443355305202</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2169,19 +2169,19 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>185.4075700059547</v>
+        <v>185.4075700260844</v>
       </c>
       <c r="C31">
-        <v>0.4510688823835424</v>
+        <v>0.451068863973196</v>
       </c>
       <c r="D31">
-        <v>15130.23808846203</v>
+        <v>15130.23808819391</v>
       </c>
       <c r="E31">
-        <v>9.581853974120978</v>
+        <v>9.581853628560548</v>
       </c>
       <c r="F31">
-        <v>32.36882367391836</v>
+        <v>32.36882369776769</v>
       </c>
     </row>
   </sheetData>
@@ -2222,19 +2222,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>148.7728158059232</v>
+        <v>148.7728157974556</v>
       </c>
       <c r="C2">
-        <v>0.2719587506648435</v>
+        <v>0.2719587492080434</v>
       </c>
       <c r="D2">
-        <v>15937.81602214246</v>
+        <v>15937.81602226501</v>
       </c>
       <c r="E2">
-        <v>5.355636026364772</v>
+        <v>5.355635959118988</v>
       </c>
       <c r="F2">
-        <v>29.77731325961316</v>
+        <v>29.77731326346695</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2242,19 +2242,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>165.4088171828183</v>
+        <v>165.4088171828213</v>
       </c>
       <c r="C3">
-        <v>0.8306008136171964</v>
+        <v>0.8306008244624195</v>
       </c>
       <c r="D3">
-        <v>14908.26980383353</v>
+        <v>14908.26980383345</v>
       </c>
       <c r="E3">
-        <v>19.95936038565265</v>
+        <v>19.95936026976447</v>
       </c>
       <c r="F3">
-        <v>79.47721395551231</v>
+        <v>79.4772139555611</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2262,19 +2262,19 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>169.8869719977172</v>
+        <v>169.886972032396</v>
       </c>
       <c r="C4">
-        <v>0.5211853320648252</v>
+        <v>0.5211853003680119</v>
       </c>
       <c r="D4">
-        <v>15214.91382609887</v>
+        <v>15214.91382540463</v>
       </c>
       <c r="E4">
-        <v>11.89850036940757</v>
+        <v>11.89850021527309</v>
       </c>
       <c r="F4">
-        <v>27.62383794212601</v>
+        <v>27.62383799898492</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2282,19 +2282,19 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>169.1796632383494</v>
+        <v>169.1796632298992</v>
       </c>
       <c r="C5">
-        <v>0.2894313329574456</v>
+        <v>0.2894313325086658</v>
       </c>
       <c r="D5">
-        <v>16034.68506609288</v>
+        <v>16034.685066274</v>
       </c>
       <c r="E5">
-        <v>6.819816139527267</v>
+        <v>6.819816129406231</v>
       </c>
       <c r="F5">
-        <v>27.7657120352349</v>
+        <v>27.76571195182325</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2302,19 +2302,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>143.8099814978865</v>
+        <v>143.8099814944561</v>
       </c>
       <c r="C6">
-        <v>0.7546577738831419</v>
+        <v>0.7546577771188072</v>
       </c>
       <c r="D6">
-        <v>15858.08158683753</v>
+        <v>15858.08158689439</v>
       </c>
       <c r="E6">
-        <v>18.55253102401521</v>
+        <v>18.55252987661336</v>
       </c>
       <c r="F6">
-        <v>56.94937678234369</v>
+        <v>56.94937547122048</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2322,19 +2322,19 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>166.9517347415309</v>
+        <v>166.9517347422215</v>
       </c>
       <c r="C7">
-        <v>0.2528263290849384</v>
+        <v>0.252826348010913</v>
       </c>
       <c r="D7">
-        <v>16143.6755069063</v>
+        <v>16143.67550687519</v>
       </c>
       <c r="E7">
-        <v>6.004006709211868</v>
+        <v>6.00400691592488</v>
       </c>
       <c r="F7">
-        <v>5.603622704208515</v>
+        <v>5.603622703002652</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2342,19 +2342,19 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>179.5564952413458</v>
+        <v>179.5564953395187</v>
       </c>
       <c r="C8">
-        <v>0.9637956249433243</v>
+        <v>0.9637955571148</v>
       </c>
       <c r="D8">
-        <v>15616.72950422728</v>
+        <v>15616.72950197944</v>
       </c>
       <c r="E8">
-        <v>22.87911183024431</v>
+        <v>22.87911134313798</v>
       </c>
       <c r="F8">
-        <v>95.99740025151375</v>
+        <v>95.9974002234573</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2362,19 +2362,19 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>173.4101299338991</v>
+        <v>173.4101299338987</v>
       </c>
       <c r="C9">
-        <v>0.1377423415689367</v>
+        <v>0.1377423309523669</v>
       </c>
       <c r="D9">
-        <v>16078.54216667756</v>
+        <v>16078.54216667757</v>
       </c>
       <c r="E9">
-        <v>3.202451573761848</v>
+        <v>3.202451335492398</v>
       </c>
       <c r="F9">
-        <v>1.511725798624033</v>
+        <v>1.511725798622379</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2382,19 +2382,19 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>165.7704306813911</v>
+        <v>165.7704306484215</v>
       </c>
       <c r="C10">
-        <v>0.7468670990625069</v>
+        <v>0.746867160577393</v>
       </c>
       <c r="D10">
-        <v>16538.86811507254</v>
+        <v>16538.86811586619</v>
       </c>
       <c r="E10">
-        <v>17.86289075094046</v>
+        <v>17.86289224695968</v>
       </c>
       <c r="F10">
-        <v>25.42382718164656</v>
+        <v>25.42382714522305</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2402,19 +2402,19 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>171.3828885168632</v>
+        <v>171.3828885339421</v>
       </c>
       <c r="C11">
-        <v>0.1321948931877392</v>
+        <v>0.1321948742788109</v>
       </c>
       <c r="D11">
-        <v>16154.01072999247</v>
+        <v>16154.01072956353</v>
       </c>
       <c r="E11">
-        <v>3.135705322478655</v>
+        <v>3.135705052553368</v>
       </c>
       <c r="F11">
-        <v>2.194921546229098</v>
+        <v>2.194921548647466</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2422,19 +2422,19 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>156.8750128124319</v>
+        <v>156.8750128896115</v>
       </c>
       <c r="C12">
-        <v>1.480408136774824</v>
+        <v>1.480408348918061</v>
       </c>
       <c r="D12">
-        <v>15205.16000130763</v>
+        <v>15205.15999929588</v>
       </c>
       <c r="E12">
-        <v>35.97917677499965</v>
+        <v>35.97918055594457</v>
       </c>
       <c r="F12">
-        <v>86.29141822476105</v>
+        <v>86.29141775365761</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2442,19 +2442,19 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>178.3250862037348</v>
+        <v>178.3250862243611</v>
       </c>
       <c r="C13">
-        <v>0.3341267732215457</v>
+        <v>0.3341267538510978</v>
       </c>
       <c r="D13">
-        <v>15779.44685710342</v>
+        <v>15779.44685674754</v>
       </c>
       <c r="E13">
-        <v>6.787946645648867</v>
+        <v>6.78794624285816</v>
       </c>
       <c r="F13">
-        <v>20.96319371273495</v>
+        <v>20.96319371478853</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2462,19 +2462,19 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>157.9754119344513</v>
+        <v>157.9754119514817</v>
       </c>
       <c r="C14">
-        <v>0.9933401362131968</v>
+        <v>0.993340136301626</v>
       </c>
       <c r="D14">
-        <v>15159.60250607362</v>
+        <v>15159.60250531826</v>
       </c>
       <c r="E14">
-        <v>24.41119286592705</v>
+        <v>24.41119286380244</v>
       </c>
       <c r="F14">
-        <v>117.7058746011468</v>
+        <v>117.7058746011431</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2482,19 +2482,19 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>160.5011110619301</v>
+        <v>160.5011110289414</v>
       </c>
       <c r="C15">
-        <v>0.7184710217042355</v>
+        <v>0.7184710327884815</v>
       </c>
       <c r="D15">
-        <v>15994.55606034038</v>
+        <v>15994.55606085495</v>
       </c>
       <c r="E15">
-        <v>14.56178897845465</v>
+        <v>14.56178927870142</v>
       </c>
       <c r="F15">
-        <v>66.29818886900962</v>
+        <v>66.29818895875623</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2502,19 +2502,19 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>164.5751922647125</v>
+        <v>164.5751922491498</v>
       </c>
       <c r="C16">
-        <v>0.7329542676741289</v>
+        <v>0.732954234756249</v>
       </c>
       <c r="D16">
-        <v>15749.8584794885</v>
+        <v>15749.85847978787</v>
       </c>
       <c r="E16">
-        <v>17.57529941056098</v>
+        <v>17.57529936373571</v>
       </c>
       <c r="F16">
-        <v>14.51835706905963</v>
+        <v>14.51835710932639</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2522,19 +2522,19 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>141.8461234250033</v>
+        <v>141.846123463497</v>
       </c>
       <c r="C17">
-        <v>0.9738966021656682</v>
+        <v>0.9738966072917437</v>
       </c>
       <c r="D17">
-        <v>15690.97998240932</v>
+        <v>15690.97998127978</v>
       </c>
       <c r="E17">
-        <v>21.87245019712299</v>
+        <v>21.87245160951602</v>
       </c>
       <c r="F17">
-        <v>82.05830601358429</v>
+        <v>82.05830601361413</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2542,19 +2542,19 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>155.7781549841492</v>
+        <v>155.7781550042425</v>
       </c>
       <c r="C18">
-        <v>0.6314216249239892</v>
+        <v>0.631421620950365</v>
       </c>
       <c r="D18">
-        <v>15325.38580258658</v>
+        <v>15325.38580210501</v>
       </c>
       <c r="E18">
-        <v>13.17697175731321</v>
+        <v>13.17697164090563</v>
       </c>
       <c r="F18">
-        <v>250.3363483965021</v>
+        <v>250.3363482996323</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2562,19 +2562,19 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>165.1476268819563</v>
+        <v>165.1476269163749</v>
       </c>
       <c r="C19">
-        <v>0.6861747494556213</v>
+        <v>0.6861747490133474</v>
       </c>
       <c r="D19">
-        <v>15922.20797017926</v>
+        <v>15922.20796962471</v>
       </c>
       <c r="E19">
-        <v>12.98358082892571</v>
+        <v>12.98358080578496</v>
       </c>
       <c r="F19">
-        <v>130.5701028813232</v>
+        <v>130.5701023786294</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2582,19 +2582,19 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>164.7058704298952</v>
+        <v>164.7058704454235</v>
       </c>
       <c r="C20">
-        <v>0.8290547280556451</v>
+        <v>0.8290548228951989</v>
       </c>
       <c r="D20">
-        <v>15184.59665895414</v>
+        <v>15184.59665808668</v>
       </c>
       <c r="E20">
-        <v>20.28595492670923</v>
+        <v>20.28595617622818</v>
       </c>
       <c r="F20">
-        <v>70.60057362932754</v>
+        <v>70.60057390905553</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2602,19 +2602,19 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>179.6377450037445</v>
+        <v>179.6377450103332</v>
       </c>
       <c r="C21">
-        <v>0.1983215374743597</v>
+        <v>0.1983215355602654</v>
       </c>
       <c r="D21">
-        <v>15865.87017857428</v>
+        <v>15865.87017842654</v>
       </c>
       <c r="E21">
-        <v>4.676971678754591</v>
+        <v>4.676971580715826</v>
       </c>
       <c r="F21">
-        <v>9.824487250897521</v>
+        <v>9.824487311422853</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2622,19 +2622,19 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>155.4793721649836</v>
+        <v>155.4793721912298</v>
       </c>
       <c r="C22">
-        <v>0.4841477609451839</v>
+        <v>0.484147763829139</v>
       </c>
       <c r="D22">
-        <v>15196.76540709554</v>
+        <v>15196.76540688962</v>
       </c>
       <c r="E22">
-        <v>11.14613092300534</v>
+        <v>11.14613098713074</v>
       </c>
       <c r="F22">
-        <v>72.98068516386719</v>
+        <v>72.98068600900432</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2642,19 +2642,19 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>167.7921780539122</v>
+        <v>167.7921781736437</v>
       </c>
       <c r="C23">
-        <v>1.125859055553025</v>
+        <v>1.125859084481209</v>
       </c>
       <c r="D23">
-        <v>15974.78239207278</v>
+        <v>15974.78238936557</v>
       </c>
       <c r="E23">
-        <v>26.3836403224815</v>
+        <v>26.38364129757253</v>
       </c>
       <c r="F23">
-        <v>135.7613898898466</v>
+        <v>135.7613898898537</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2662,19 +2662,19 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>164.1497487563155</v>
+        <v>164.1497489768931</v>
       </c>
       <c r="C24">
-        <v>1.211485916399542</v>
+        <v>1.211485918408979</v>
       </c>
       <c r="D24">
-        <v>15748.2754066314</v>
+        <v>15748.27540128122</v>
       </c>
       <c r="E24">
-        <v>29.76856243960366</v>
+        <v>29.76856243896027</v>
       </c>
       <c r="F24">
-        <v>47.62633976731833</v>
+        <v>47.62633977446727</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2682,19 +2682,19 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>159.7076029903515</v>
+        <v>159.7076030166918</v>
       </c>
       <c r="C25">
-        <v>0.2634195167477817</v>
+        <v>0.2634195273608695</v>
       </c>
       <c r="D25">
-        <v>15429.0327509008</v>
+        <v>15429.03275082562</v>
       </c>
       <c r="E25">
-        <v>6.234251868585819</v>
+        <v>6.234251733533818</v>
       </c>
       <c r="F25">
-        <v>33.25067693706753</v>
+        <v>33.25067693706743</v>
       </c>
     </row>
   </sheetData>

</xml_diff>